<commit_message>
replaced myoutput with correct version
</commit_message>
<xml_diff>
--- a/Output/KeywordIdentification/Test Set of 50 Group Folders/TotalCircnew_myoutput.xlsx
+++ b/Output/KeywordIdentification/Test Set of 50 Group Folders/TotalCircnew_myoutput.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="49">
   <si>
     <t>Keywords</t>
   </si>
@@ -43,21 +43,21 @@
     <t>return on invested capital</t>
   </si>
   <si>
+    <t>irr</t>
+  </si>
+  <si>
+    <t>cost of debt</t>
+  </si>
+  <si>
+    <t>discount rate</t>
+  </si>
+  <si>
     <t>occ</t>
   </si>
   <si>
     <t>interest rate</t>
   </si>
   <si>
-    <t>irr</t>
-  </si>
-  <si>
-    <t>discount rate</t>
-  </si>
-  <si>
-    <t>cost of debt</t>
-  </si>
-  <si>
     <t>2020-10-01</t>
   </si>
   <si>
@@ -70,12 +70,18 @@
     <t>BURFORD CAPITAL LTD</t>
   </si>
   <si>
+    <t>KONECRANES PLC</t>
+  </si>
+  <si>
+    <t>TANZANIA MINERALS CORP</t>
+  </si>
+  <si>
+    <t>NOVAGOLD RESOURCES INC.</t>
+  </si>
+  <si>
     <t>MENLO THERAPEUTICS INC</t>
   </si>
   <si>
-    <t>TANZANIA MINERALS CORP</t>
-  </si>
-  <si>
     <t>CONAGRA BRANDS INC</t>
   </si>
   <si>
@@ -88,21 +94,21 @@
     <t>WEEDMD INC</t>
   </si>
   <si>
-    <t>KONECRANES PLC</t>
-  </si>
-  <si>
-    <t>NOVAGOLD RESOURCES INC.</t>
-  </si>
-  <si>
     <t>BURF.L - Event Transcript of Burford Capital Ltd conference call, Oct. 01, 2020 / 9:00AM ET</t>
   </si>
   <si>
+    <t>KCRA.HE - Event Transcript of Konecranes Abp conference call, Oct. 01, 2020 / 2:30AM ET</t>
+  </si>
+  <si>
+    <t>JUSH.CD - Event Transcript of Jushi Holdings Inc conference call, Oct. 01, 2020 / 10:00AM ET</t>
+  </si>
+  <si>
+    <t>NG.A - Event Transcript of NovaGold Resources Inc conference call, Oct. 01, 2020 / 11:00AM ET</t>
+  </si>
+  <si>
     <t>VYNE.OQ - Event Transcript of Vyne Therapeutics Inc conference call, Oct. 01, 2020 / 12:00PM ET</t>
   </si>
   <si>
-    <t>JUSH.CD - Event Transcript of Jushi Holdings Inc conference call, Oct. 01, 2020 / 10:00AM ET</t>
-  </si>
-  <si>
     <t>CAG.N - Event Transcript of Conagra Brands Inc conference call, Oct. 01, 2020 / 9:30AM ET</t>
   </si>
   <si>
@@ -121,15 +127,18 @@
     <t>WMD.V - Event Transcript of WeedMD Inc conference call, Oct. 01, 2020 / 10:00AM ET</t>
   </si>
   <si>
-    <t>KCRA.HE - Event Transcript of Konecranes Abp conference call, Oct. 01, 2020 / 2:30AM ET</t>
-  </si>
-  <si>
-    <t>NG.A - Event Transcript of NovaGold Resources Inc conference call, Oct. 01, 2020 / 11:00AM ET</t>
-  </si>
-  <si>
     <t>Looking just at one group of related cases, we produced $423 million in group realizations. That's a 56% IRR on those investments, return on invested capital of 194%. And that just feeds into what is now an 11-year track record at Burford. And within that track record, we've now generated more than $1.6 billion of investment recoveries and that is in our core litigation finance business. That's not including any of the other adjacent strategies like complex strategies, for example, that we also run. And on that $1.6 billion, across 11 years, we've produced very consistent IRRs right now at 32%. And our returns -- our nominal returns actually went up to 97% return on invested capital. And so to underline the point that this is the way this business works, this combination of settlements and outsized wins accompanied by a few losses, we now have 23 separate investments in our history that have produced more than a 200% return on invested capital. And we've done all</t>
   </si>
   <si>
+    <t>The name of the future company will also be determined and announced at a later stage. And I think it's very, very important to note that both Boards of Directors have unanimously recommended this merger. In addition, we have irrevocable votes to vote in favor of this merger in both companies, represented from the shareholders in both companies. From the Cargotec side, 44.8% of the shares and 76.3% of the votes are irrevocably committed to taking this merger. And from the Konecranes side, 27.4% already of the votes and the shares are irrevocably committed to taking this step together.  This is how we're going to make the merger happen. This is such that Konecranes shall be statutorily merged into Cargotec. And to make that happen prior to the combination, Cargotec will split its A shares and its B shares on a 3:1 basis. In addition, in advance of the combination, Konecranes will propose to its AGM in 2021 an extra dividend of profits at EUR 2 per share. The new shares will be shared with Konecranes shareholders in a mechanism such that 50% of the shares and votes of the new company will be held by current Konecranes shareholders and by Cargotec shareholders, making the 50-50 split that you see here.</t>
+  </si>
+  <si>
+    <t>James Anthony Cacioppo - Jushi Holdings Inc. - Founder, Chairman &amp; CEO Yes. And I'll add to that. I think what Kim talked about is completely valid and very detailed and as you can tell, we manage all aspects of the operation to a high degree of precision. But I also believe that on an operating basis, the biggest upticks will take place by allowing credit cards to being used in dispensaries, if it was federal and ATM cards and that would -- that there's -- we have quantitative data that tells us that there's a meaningful impact, double-digit percent impact and I don't want to get any more specific than that, off the top of my head, but we have meaningful data on that, that, that will drive sales, not just for us, but obviously, the industry. The other big factor that would cause your overall net income margin to go up is your cost of debt, I think, would go down quite dramatically. You are -- if you look in Massachusetts, there are banks loaning to the industry. And I'm not sure what's behind that because we're not in Massachusetts. I'm not sure if some of these private companies have personal guarantees or whatever it is. But they're doing it around the 6% level. And if you look at the cost of debt now, you could look at Curaleaf's deal, I think that trades at like a yield to first call at like 11%, yield to first call, yield to worst. And if you look at that, and if you look at getting bank debt at 6%, would bring down your cost of debt quite dramatically. And Cura, it has the cheapest cost of debt, I would imagine. And so some people are paying dramatically more than that, mid- to high teens. So I think the cost of debt will go way down. And I think it will be huge -- and for the industry. And we hope it happens in one way. But in the other way, if it doesn't happen, we have an advantage in being able to buy assets from a more capital constrained industry.</t>
+  </si>
+  <si>
+    <t>Next. For me and for our investors, we want the leverage to that higher gold price. But we want to be in a place that will allow us to keep it, that won't turn around and say, "Hey, you're making a windfall. We want part of that." The leverage provided by NovaGold and by Donlin, for us and for Barrick, is absolutely gorgeous. I do believe that at $2,000 gold, this is a $20 billion asset. We haven't even spoken about optimization. This is not adding potentially more reserves or any other upsides. That's just merely a function of the fact that I think that very, very scarce North American assets of high-quality size that moves the needle will be valued using 0% discount rates, especially if they have any exploration potential, and I don't believe anyone has more exploration potential than Donlin.  Next. One of the beautiful things, as I mentioned, about NovaGold is that in addition to having a lot of cash where we don't need to raise more money, we have a really, really, really interesting and smart investor base. And as more people are asking for brokers to give them exposure to assets which are located in places that potentially they'd be willing to take their kids. Alaska with whale watching and salmon fishing falls into that category. Australia, the Great Barrier Reef. Nevada, you've got gambling, you've got all the other fun things for the family in different places. You'd be surprised, but the premium rating will be given for those assets which are in places where investors' ICs would say, "If you're going to go on a mine tour, are you willing to go there?" And definitely, Donlin falls within that category. But more than that, when they look at our shareholder base, what they're going to see is very, very smart money. And some of those new investors are already starting to call up these people and say, "Hey, can you tell us more about this?" And pretty much what they're hearing is that Donlin is unique, and this is a pure-play on what will be, hopefully, the largest pure gold mine in the world over the course of time.</t>
+  </si>
+  <si>
     <t>Next slide, please. So Dr. Lain covered this very thoroughly. The historical treatment paradigm, typically and this is a very sort of abbreviated view. For the mild patient, typically will use topicals and those topicals can be prescription or over the counter. When we move into that moderate patient, the oral medication, certainly will be an option via antibiotics or spironolactone and some orals as well as prescription topicals. Now when we move to severe, certainly, we're going to use oral medications as well as prescription topicals as well as potentially oral isotretinoin. Next slide, please. So relative to the epidemiology of acne in the United States, roughly 50 million people suffer with acne vulgaris. And It can affect roughly 85% of teenagers that can occur at most ages and even persistent to adulthood. It's associated with a significant amount of physical as well as psychological morbidity, including permanent scarring of the skin as well as poor self image and self esteem issues as well as depression and anxiety. And we'll talk a little about that as I they have 1 patient who exhibited some of these effects, we'll show that later on. And then relative to its direct impact relative to cost and indirect cost, totals roughly $3 billion. So folks, we have a captive audience. And to have AMZEEQ this novel minocycline foam formulation in our therapeutic armamentarium is most certainly beneficial. Next slide, please. Okay. So Dr. Lain again covered this very thoroughly. Relative to efficacy, our Phase III clinical trials showed fantastic results and relative to systemic exposure. Kudos to VYNE for a very good study looking at maximum use where they essentially compared oral minocycline at 1 mg per kilogram versus topical minocycline at 4 grams topically daily for 21 days, which is actually 8x the dose that we use AMZEEQ, so much more powerful for their maximum use study. And they assessed the serum concentrations comparatively between the oral administration and the topical, and there was a 750 fold decrease in the topical versus oral. So taking it orally, certainly the systemic absorption is much more and that sort of plays well into its safety profile. So it's a minimal adverse event profile. And essentially, what we looked at, as Dr. Lain tried to was was the redness to irritation, skin peeling, burning, hyperpigmentation, which are all I'll tell you a teetering in the acne space.</t>
   </si>
   <si>
@@ -152,15 +161,6 @@
   </si>
   <si>
     <t>Greg McLeish - Mackie Research Capital Corporation, Research Division - Director &amp; Analyst of Special Situations Well, I guess my concern here is that you're continuing to burn through cash. You've got the new LiUNA credit line, which is -- given it's at 15% interest rates, I mean that's $4.5 million per year. Now I know you can do a payment in kind, but what my concern is, is that you're going to absolutely dilute the equity shareholders going forward because you've got a high debt position. And when the share price is where it is, it's hard to raise equity at these levels. So what comfort can you give to the equity shareholders of the business that you can generate a long-term return for them? Lincoln E. C. Greenidge - WeedMD Inc. - CFO So I think I'll take that. And if Angelo or Stephen want to add some color, they can certainly do so afterwards. I'll reiterate that the comfort I give certainly shareholders in terms of not diluting the interest is that we will become cash positive, and we will be able to service our debt. The plans that we have in terms of automation, we'll continue to automate. We'll continue to look at all our costs and reduce. And I'm seeing the signs right now as we go into, I guess, at Q4 now that we can reduce our costs significantly in order to -- continue to reach to that -- meet our plan. And that plan is obviously to become a sustainable, profitable business.</t>
-  </si>
-  <si>
-    <t>The name of the future company will also be determined and announced at a later stage. And I think it's very, very important to note that both Boards of Directors have unanimously recommended this merger. In addition, we have irrevocable votes to vote in favor of this merger in both companies, represented from the shareholders in both companies. From the Cargotec side, 44.8% of the shares and 76.3% of the votes are irrevocably committed to taking this merger. And from the Konecranes side, 27.4% already of the votes and the shares are irrevocably committed to taking this step together.  This is how we're going to make the merger happen. This is such that Konecranes shall be statutorily merged into Cargotec. And to make that happen prior to the combination, Cargotec will split its A shares and its B shares on a 3:1 basis. In addition, in advance of the combination, Konecranes will propose to its AGM in 2021 an extra dividend of profits at EUR 2 per share. The new shares will be shared with Konecranes shareholders in a mechanism such that 50% of the shares and votes of the new company will be held by current Konecranes shareholders and by Cargotec shareholders, making the 50-50 split that you see here.</t>
-  </si>
-  <si>
-    <t>Next. For me and for our investors, we want the leverage to that higher gold price. But we want to be in a place that will allow us to keep it, that won't turn around and say, "Hey, you're making a windfall. We want part of that." The leverage provided by NovaGold and by Donlin, for us and for Barrick, is absolutely gorgeous. I do believe that at $2,000 gold, this is a $20 billion asset. We haven't even spoken about optimization. This is not adding potentially more reserves or any other upsides. That's just merely a function of the fact that I think that very, very scarce North American assets of high-quality size that moves the needle will be valued using 0% discount rates, especially if they have any exploration potential, and I don't believe anyone has more exploration potential than Donlin.  Next. One of the beautiful things, as I mentioned, about NovaGold is that in addition to having a lot of cash where we don't need to raise more money, we have a really, really, really interesting and smart investor base. And as more people are asking for brokers to give them exposure to assets which are located in places that potentially they'd be willing to take their kids. Alaska with whale watching and salmon fishing falls into that category. Australia, the Great Barrier Reef. Nevada, you've got gambling, you've got all the other fun things for the family in different places. You'd be surprised, but the premium rating will be given for those assets which are in places where investors' ICs would say, "If you're going to go on a mine tour, are you willing to go there?" And definitely, Donlin falls within that category. But more than that, when they look at our shareholder base, what they're going to see is very, very smart money. And some of those new investors are already starting to call up these people and say, "Hey, can you tell us more about this?" And pretty much what they're hearing is that Donlin is unique, and this is a pure-play on what will be, hopefully, the largest pure gold mine in the world over the course of time.</t>
-  </si>
-  <si>
-    <t>James Anthony Cacioppo - Jushi Holdings Inc. - Founder, Chairman &amp; CEO Yes. And I'll add to that. I think what Kim talked about is completely valid and very detailed and as you can tell, we manage all aspects of the operation to a high degree of precision. But I also believe that on an operating basis, the biggest upticks will take place by allowing credit cards to being used in dispensaries, if it was federal and ATM cards and that would -- that there's -- we have quantitative data that tells us that there's a meaningful impact, double-digit percent impact and I don't want to get any more specific than that, off the top of my head, but we have meaningful data on that, that, that will drive sales, not just for us, but obviously, the industry. The other big factor that would cause your overall net income margin to go up is your cost of debt, I think, would go down quite dramatically. You are -- if you look in Massachusetts, there are banks loaning to the industry. And I'm not sure what's behind that because we're not in Massachusetts. I'm not sure if some of these private companies have personal guarantees or whatever it is. But they're doing it around the 6% level. And if you look at the cost of debt now, you could look at Curaleaf's deal, I think that trades at like a yield to first call at like 11%, yield to first call, yield to worst. And if you look at that, and if you look at getting bank debt at 6%, would bring down your cost of debt quite dramatically. And Cura, it has the cheapest cost of debt, I would imagine. And so some people are paying dramatically more than that, mid- to high teens. So I think the cost of debt will go way down. And I think it will be huge -- and for the industry. And we hope it happens in one way. But in the other way, if it doesn't happen, we have an advantage in being able to buy assets from a more capital constrained industry.</t>
   </si>
 </sst>
 </file>
@@ -518,7 +518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -578,7 +578,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
         <v>14</v>
@@ -610,7 +610,7 @@
         <v>14</v>
       </c>
       <c r="C4">
-        <v>70489054</v>
+        <v>70488207</v>
       </c>
       <c r="D4" t="s">
         <v>15</v>
@@ -630,7 +630,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
         <v>14</v>
@@ -656,13 +656,13 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
       </c>
       <c r="C6">
-        <v>70486677</v>
+        <v>70487273</v>
       </c>
       <c r="D6" t="s">
         <v>15</v>
@@ -682,13 +682,13 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
       </c>
       <c r="C7">
-        <v>70487360</v>
+        <v>70489054</v>
       </c>
       <c r="D7" t="s">
         <v>15</v>
@@ -697,7 +697,7 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G7" t="s">
         <v>30</v>
@@ -708,13 +708,13 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B8" t="s">
         <v>14</v>
       </c>
       <c r="C8">
-        <v>70487355</v>
+        <v>70488559</v>
       </c>
       <c r="D8" t="s">
         <v>15</v>
@@ -723,10 +723,10 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="H8" t="s">
         <v>42</v>
@@ -734,13 +734,13 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B9" t="s">
         <v>14</v>
       </c>
       <c r="C9">
-        <v>70488831</v>
+        <v>70486677</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -749,10 +749,10 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H9" t="s">
         <v>43</v>
@@ -760,13 +760,13 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>14</v>
       </c>
       <c r="C10">
-        <v>70489054</v>
+        <v>70487360</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -775,24 +775,24 @@
         <v>16</v>
       </c>
       <c r="F10" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="H10" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
         <v>14</v>
       </c>
       <c r="C11">
-        <v>70488559</v>
+        <v>70487355</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -801,24 +801,24 @@
         <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G11" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H11" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:8">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
       <c r="C12">
-        <v>70486677</v>
+        <v>70488831</v>
       </c>
       <c r="D12" t="s">
         <v>15</v>
@@ -827,24 +827,24 @@
         <v>16</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="G12" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="H12" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
         <v>14</v>
       </c>
       <c r="C13">
-        <v>70487360</v>
+        <v>70487580</v>
       </c>
       <c r="D13" t="s">
         <v>15</v>
@@ -853,24 +853,24 @@
         <v>16</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="H13" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:8">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
       </c>
       <c r="C14">
-        <v>70487355</v>
+        <v>70486735</v>
       </c>
       <c r="D14" t="s">
         <v>15</v>
@@ -879,350 +879,12 @@
         <v>16</v>
       </c>
       <c r="F14" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="G14" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
-        <v>9</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <v>70488831</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F15" t="s">
-        <v>21</v>
-      </c>
-      <c r="G15" t="s">
-        <v>32</v>
-      </c>
-      <c r="H15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <v>70487580</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="E16" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G16" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <v>70486735</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="E17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" t="s">
-        <v>34</v>
-      </c>
-      <c r="H17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>70487580</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" t="s">
-        <v>16</v>
-      </c>
-      <c r="F18" t="s">
-        <v>22</v>
-      </c>
-      <c r="G18" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>70486735</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" t="s">
-        <v>34</v>
-      </c>
-      <c r="H19" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <v>70486599</v>
-      </c>
-      <c r="D20" t="s">
-        <v>15</v>
-      </c>
-      <c r="E20" t="s">
-        <v>16</v>
-      </c>
-      <c r="F20" t="s">
-        <v>17</v>
-      </c>
-      <c r="G20" t="s">
-        <v>26</v>
-      </c>
-      <c r="H20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21">
-        <v>70488207</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="E21" t="s">
-        <v>16</v>
-      </c>
-      <c r="F21" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>70486599</v>
-      </c>
-      <c r="D22" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" t="s">
-        <v>16</v>
-      </c>
-      <c r="F22" t="s">
-        <v>17</v>
-      </c>
-      <c r="G22" t="s">
-        <v>26</v>
-      </c>
-      <c r="H22" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
-        <v>11</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23">
-        <v>70488207</v>
-      </c>
-      <c r="D23" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" t="s">
-        <v>16</v>
-      </c>
-      <c r="F23" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24">
-        <v>70487273</v>
-      </c>
-      <c r="D24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
-        <v>12</v>
-      </c>
-      <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25">
-        <v>70487273</v>
-      </c>
-      <c r="D25" t="s">
-        <v>15</v>
-      </c>
-      <c r="E25" t="s">
-        <v>16</v>
-      </c>
-      <c r="F25" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
-        <v>13</v>
-      </c>
-      <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26">
-        <v>70488559</v>
-      </c>
-      <c r="D26" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8">
-      <c r="A27" t="s">
-        <v>13</v>
-      </c>
-      <c r="B27" t="s">
-        <v>14</v>
-      </c>
-      <c r="C27">
-        <v>70488559</v>
-      </c>
-      <c r="D27" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>